<commit_message>
Excel rename European Powers to Europe
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szymon/dev/dets-belfer-15-may/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAB0C135-17E3-6943-AD1C-4941D17E3564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E76D2-E7FB-254C-9234-FA006E2C3C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39040" windowHeight="21040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="63">
   <si>
     <t>AI</t>
   </si>
@@ -228,6 +228,9 @@
   <si>
     <t>U.A.E.</t>
   </si>
+  <si>
+    <t>Europe</t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -379,6 +382,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1367,13 +1371,13 @@
         <f t="array" ref="D27">INDEX(Semicon!#REF!, MATCH(Summary!A27, Semicon!$A$2:$A$27, 0))</f>
         <v>#REF!</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="4" t="e">
         <f t="array" ref="E27">INDEX(Space!$B$2:$B$27, MATCH(Summary!A27, Space!$A$2:$A$27, 0))</f>
-        <v>4.6630220293689222</v>
-      </c>
-      <c r="F27" s="4">
+        <v>#N/A</v>
+      </c>
+      <c r="F27" s="4" t="e">
         <f t="array" ref="F27">INDEX(Quantum!$B$2:$B$27, MATCH(Summary!A27, Quantum!$A$2:$A$27, 0))</f>
-        <v>5.6687535638702542</v>
+        <v>#N/A</v>
       </c>
       <c r="G27" s="4" t="e">
         <f t="shared" si="0"/>
@@ -2363,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I998"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3136,8 +3140,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>28</v>
+      <c r="A27" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="18">
         <v>0.14638221241520169</v>
@@ -4146,7 +4150,7 @@
   <dimension ref="A1:J998"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:J27"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4988,8 +4992,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>28</v>
+      <c r="A27" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="16">
         <v>0.45025700216234282</v>
@@ -6001,7 +6005,7 @@
   <dimension ref="A1:J998"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:J27"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6842,8 +6846,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>28</v>
+      <c r="A27" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="18">
         <v>0.2019005584557757</v>
@@ -7855,7 +7859,7 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8852,8 +8856,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>28</v>
+      <c r="A27" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="15">
         <v>4.6630220293689222</v>
@@ -9870,8 +9874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J998"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10722,8 +10726,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>28</v>
+      <c r="A27" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="9">
         <v>5.6687535638702542</v>

</xml_diff>